<commit_message>
Generación de Checklist Organizacional
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/Checklist_Organizacional_150616.xlsx
+++ b/qualtcom/Organizacional/Calidad/Checklist_Organizacional_150616.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\qtp\qualtcom\Organizacional\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\qtp\qualtcom\Organizacional\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Checklist de Auditorías</t>
   </si>
@@ -216,13 +216,16 @@
     <t>¿Se reviso el esfuerzo planeado y real?</t>
   </si>
   <si>
-    <t>Samuel Reyna</t>
-  </si>
-  <si>
     <t>Junio 16, 2015</t>
   </si>
   <si>
     <t>Mayra Tejeda Hernández</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -340,8 +343,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +398,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB3B3B3"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,14 +553,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -645,9 +675,17 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1025,7 +1063,7 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:F7"/>
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1067,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="58"/>
@@ -1078,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="58"/>
       <c r="E6" s="58"/>
@@ -1088,12 +1126,12 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1">
       <c r="B10" s="2" t="s">
@@ -1135,11 +1173,11 @@
       </c>
       <c r="C13" s="8">
         <f>COUNTA(Procesos!C11:C14)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="10" t="e">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10">
         <f>COUNTIF((Procesos!C11:C14),"x")/(COUNTIF((Procesos!C11:C14),"x")+COUNTIF((Procesos!D11:D14),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" customHeight="1">
@@ -1182,11 +1220,11 @@
       </c>
       <c r="C18" s="8">
         <f>COUNTA(Productos!D11:D17)</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="10" t="e">
+        <v>7</v>
+      </c>
+      <c r="D18" s="10">
         <f>COUNTIF((Productos!D11:D17),"x")/(COUNTIF((Productos!D11:D17),"x")+COUNTIF((Productos!E11:E17),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16.5" customHeight="1">
@@ -1196,11 +1234,11 @@
       </c>
       <c r="C19" s="8">
         <f>COUNTA(Productos!D19:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="10" t="e">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10">
         <f>COUNTIF((Productos!D19:D25),"x")/(COUNTIF((Productos!D19:D25),"x")+COUNTIF((Productos!E19:E25),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="19.5" customHeight="1">
@@ -1210,11 +1248,11 @@
       </c>
       <c r="C20" s="8">
         <f>COUNTA(Productos!D27:D32)</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="10" t="e">
+        <v>6</v>
+      </c>
+      <c r="D20" s="10">
         <f>COUNTIF((Productos!D27:D32),"x")/(COUNTIF((Productos!D27:D32),"x")+COUNTIF((Productos!E27:E32),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1228,7 +1266,7 @@
     <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1237,7 +1275,7 @@
   <dimension ref="A1:AMI15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1372,7 +1410,9 @@
       <c r="B11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
@@ -1383,7 +1423,9 @@
       <c r="B12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
@@ -1394,7 +1436,9 @@
       <c r="B13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
@@ -1405,7 +1449,9 @@
       <c r="B14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="23"/>
@@ -1438,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1498,10 +1544,10 @@
     </row>
     <row r="4" spans="1:8" ht="13.15" customHeight="1">
       <c r="A4" s="34"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
       <c r="F4" s="36"/>
@@ -1564,10 +1610,10 @@
       <c r="H9" s="39"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
@@ -1579,7 +1625,9 @@
       <c r="C11" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1590,7 +1638,9 @@
       <c r="C12" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="66" t="s">
+        <v>66</v>
+      </c>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
       <c r="G12" s="46"/>
@@ -1601,7 +1651,9 @@
       <c r="C13" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="23"/>
@@ -1612,7 +1664,9 @@
       <c r="C14" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="23"/>
@@ -1623,7 +1677,9 @@
       <c r="C15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="23"/>
@@ -1634,7 +1690,9 @@
       <c r="C16" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="23"/>
@@ -1645,17 +1703,19 @@
       <c r="C17" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="39"/>
     </row>
     <row r="18" spans="2:8" ht="15.75">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="43"/>
@@ -1667,7 +1727,9 @@
       <c r="C19" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="23"/>
@@ -1678,7 +1740,9 @@
       <c r="C20" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="67" t="s">
+        <v>66</v>
+      </c>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
@@ -1689,7 +1753,9 @@
       <c r="C21" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="66" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" s="46"/>
       <c r="F21" s="47"/>
       <c r="G21" s="46"/>
@@ -1700,7 +1766,9 @@
       <c r="C22" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="23"/>
@@ -1711,7 +1779,9 @@
       <c r="C23" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
@@ -1722,7 +1792,9 @@
       <c r="C24" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="23"/>
@@ -1733,17 +1805,19 @@
       <c r="C25" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="23"/>
       <c r="H25" s="39"/>
     </row>
     <row r="26" spans="2:8" ht="15.75">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="64"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
@@ -1755,7 +1829,9 @@
       <c r="C27" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="46"/>
+      <c r="D27" s="66" t="s">
+        <v>66</v>
+      </c>
       <c r="E27" s="46"/>
       <c r="F27" s="47"/>
       <c r="G27" s="46"/>
@@ -1766,7 +1842,9 @@
       <c r="C28" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="23"/>
@@ -1777,7 +1855,9 @@
       <c r="C29" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="23"/>
@@ -1788,7 +1868,9 @@
       <c r="C30" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="23"/>
@@ -1799,7 +1881,9 @@
       <c r="C31" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="23"/>
@@ -1810,15 +1894,17 @@
       <c r="C32" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="23"/>
       <c r="H32" s="38"/>
     </row>
     <row r="33" spans="2:8" ht="15.75">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
       <c r="F33" s="48"/>
@@ -1827,18 +1913,18 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1864,14 +1950,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.75">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
       <c r="H3" s="49"/>
     </row>
     <row r="4" spans="2:8" ht="36.6" customHeight="1">

</xml_diff>